<commit_message>
Fixed DieteryRecommendation to STU3, added example
</commit_message>
<xml_diff>
--- a/Mappings/DietaryRecommendations - STU3.xlsx
+++ b/Mappings/DietaryRecommendations - STU3.xlsx
@@ -8,15 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="DietaryRecommendations" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t xml:space="preserve"># </t>
   </si>
@@ -140,15 +138,9 @@
     <t>NutritionOrder.oralDiet.extension</t>
   </si>
   <si>
-    <t>Created an extension. NutritionOrder.oralDiet.instruction is used for NursingPrecedure.Activity.</t>
-  </si>
-  <si>
     <t>The VerpleegkundigeActie is defined within the NutritionOrder resource. No reference is used.</t>
   </si>
   <si>
-    <t>Not mandatory in th ZIB</t>
-  </si>
-  <si>
     <t>NutritionOrder.oralDiet.schedule.period / NutritionOrder.supplement.schedule.period / NutritionOrder.enteralFormula.administration.schedule.period</t>
   </si>
   <si>
@@ -165,13 +157,25 @@
   </si>
   <si>
     <t xml:space="preserve">Beceause this ZIB DietaryRecommendations belongs to the NursingBuilding blocks, the NutritionOrder resource is used. </t>
+  </si>
+  <si>
+    <t>gForge ticket #13294.                              Created an extension. NutritionOrder.oralDiet.instruction is used for NursingPrecedure.Activity.</t>
+  </si>
+  <si>
+    <t>At the moment only NutritionOrder.oralDiet is profiled</t>
+  </si>
+  <si>
+    <t>Not mandatory in th ZIB - Needed in profile?</t>
+  </si>
+  <si>
+    <t>Not mandatory in th ZIB  - The NutritionOrder is a request resource. Therfore there is no information provided on who performed the order. Needed in the profile? Not actually part of the BGZ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -213,8 +217,14 @@
       <color rgb="FF00B050"/>
       <name val="Open Sans"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,6 +243,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -412,11 +427,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
@@ -524,8 +540,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -828,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -841,7 +861,7 @@
     <col min="7" max="7" width="12" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" customWidth="1"/>
-    <col min="10" max="10" width="75.28515625" customWidth="1"/>
+    <col min="10" max="10" width="75.140625" customWidth="1"/>
     <col min="11" max="11" width="39.28515625" style="15" customWidth="1"/>
     <col min="12" max="12" width="46.42578125" customWidth="1"/>
   </cols>
@@ -932,7 +952,7 @@
       </c>
       <c r="K4" s="9"/>
     </row>
-    <row r="5" spans="1:11" ht="38.25">
+    <row r="5" spans="1:11" ht="51">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -954,7 +974,7 @@
         <v>36</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="38.25">
@@ -977,7 +997,7 @@
       </c>
       <c r="J6" s="13"/>
       <c r="K6" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1001,11 +1021,11 @@
       <c r="J7" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="K7" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="K7" s="37" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="63.75">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -1026,11 +1046,11 @@
       <c r="J8" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="38.25">
+      <c r="K8" s="37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="25.5">
       <c r="A9" s="10">
         <v>7</v>
       </c>
@@ -1049,11 +1069,11 @@
         <v>30</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K9" s="9"/>
     </row>
-    <row r="10" spans="1:11" ht="51">
+    <row r="10" spans="1:11" ht="25.5">
       <c r="A10" s="10">
         <v>8</v>
       </c>
@@ -1072,11 +1092,11 @@
         <v>31</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K10" s="9"/>
     </row>
-    <row r="11" spans="1:11" ht="38.25">
+    <row r="11" spans="1:11" ht="25.5">
       <c r="A11" s="10">
         <v>9</v>
       </c>
@@ -1095,11 +1115,11 @@
         <v>8</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K11" s="9"/>
     </row>
-    <row r="12" spans="1:11" ht="51">
+    <row r="12" spans="1:11" ht="38.25">
       <c r="A12" s="10">
         <v>10</v>
       </c>
@@ -1118,11 +1138,11 @@
         <v>5</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K12" s="9"/>
     </row>
-    <row r="13" spans="1:11" ht="51">
+    <row r="13" spans="1:11" ht="38.25">
       <c r="A13" s="16">
         <v>11</v>
       </c>
@@ -1141,13 +1161,16 @@
         <v>5</v>
       </c>
       <c r="J13" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K13" s="23"/>
     </row>
     <row r="14" spans="1:11">
+      <c r="J14" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="K14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1184,28 +1207,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated mappings and progress .xlsx
</commit_message>
<xml_diff>
--- a/Mappings/DietaryRecommendations - STU3.xlsx
+++ b/Mappings/DietaryRecommendations - STU3.xlsx
@@ -510,6 +510,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -539,9 +542,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -848,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -861,8 +861,8 @@
     <col min="7" max="7" width="12" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" customWidth="1"/>
-    <col min="10" max="10" width="75.140625" customWidth="1"/>
-    <col min="11" max="11" width="39.28515625" style="15" customWidth="1"/>
+    <col min="10" max="10" width="88.7109375" customWidth="1"/>
+    <col min="11" max="11" width="63" style="15" customWidth="1"/>
     <col min="12" max="12" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -870,15 +870,15 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
       <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
@@ -891,16 +891,16 @@
     </row>
     <row r="2" spans="1:11" ht="15">
       <c r="A2" s="3"/>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="36"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="37"/>
       <c r="J2" s="4" t="s">
         <v>32</v>
       </c>
@@ -911,12 +911,12 @@
         <v>1</v>
       </c>
       <c r="B3" s="6"/>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
       <c r="G3" t="s">
         <v>11</v>
       </c>
@@ -934,12 +934,12 @@
         <v>2</v>
       </c>
       <c r="B4" s="11"/>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
       <c r="G4" t="s">
         <v>12</v>
       </c>
@@ -957,12 +957,12 @@
         <v>3</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
       <c r="G5" t="s">
         <v>7</v>
       </c>
@@ -1021,7 +1021,7 @@
       <c r="J7" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="K7" s="37" t="s">
+      <c r="K7" s="27" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1046,7 +1046,7 @@
       <c r="J8" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="37" t="s">
+      <c r="K8" s="27" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>